<commit_message>
Dip_02 Added new cases to 'Cases' changed Plan
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Вкладка "Новости"</t>
   </si>
   <si>
-    <t>Функция кнопки "Обновить"</t>
-  </si>
-  <si>
     <t>Вкладка "О приложении"</t>
   </si>
   <si>
@@ -125,6 +122,18 @@
   </si>
   <si>
     <t>Переход по пуш-уведомлению при свёрнутом приложении</t>
+  </si>
+  <si>
+    <t>Функция кнопки сортировки</t>
+  </si>
+  <si>
+    <t>Функция кнопки фильтра</t>
+  </si>
+  <si>
+    <t>Функция кнопки создания новости</t>
+  </si>
+  <si>
+    <t>Статус</t>
   </si>
 </sst>
 </file>
@@ -167,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +201,14 @@
         <bgColor rgb="FFEAD1DC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -264,21 +279,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -296,11 +296,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -308,9 +345,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -320,11 +354,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -344,19 +384,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -569,254 +612,299 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="12.6640625" style="5"/>
+    <col min="1" max="1" width="23.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.2">
+    <row r="1" spans="1:4" ht="13.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="44.4" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="D1" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="44.4" customHeight="1">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="44.4" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:4" ht="44.4" customHeight="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="23.4" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:4" ht="23.4" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="23.4" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="4" t="s">
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:4" ht="23.4" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="42.6" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4" ht="42.6" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="42.6" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="4" t="s">
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" ht="42.6" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="39.6">
-      <c r="A8" s="12" t="s">
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="39.6">
+      <c r="A8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="26.4">
+      <c r="A9" s="14"/>
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="26.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="39.6">
+      <c r="A10" s="14"/>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="39.6">
-      <c r="A10" s="13"/>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" ht="26.4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="26.4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="6" t="s">
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" ht="13.2">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="13.2">
-      <c r="A12" s="12" t="s">
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="13.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="13.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="13.2">
+      <c r="A15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="13.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="26.4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="26.4">
+      <c r="A18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="26.4">
+      <c r="A19" s="15"/>
+      <c r="B19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" ht="26.4">
+      <c r="A20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="C20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" ht="31.8" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="13.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="39" customHeight="1">
+      <c r="A22" s="9"/>
+      <c r="B22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="13.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="13.2">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="26.4">
-      <c r="A16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="26.4">
-      <c r="A17" s="14"/>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="26.4">
-      <c r="A18" s="15" t="s">
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" ht="51" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.8" customHeight="1">
-      <c r="A19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="39" customHeight="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="51" customHeight="1">
-      <c r="A21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" ht="42.6" customHeight="1">
+      <c r="A24" s="9"/>
+      <c r="B24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="42.6" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="45.6" customHeight="1"/>
+      <c r="C24" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="27" spans="1:4" ht="45.6" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A19:A20"/>
+  <mergeCells count="9">
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C22">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C24">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>